<commit_message>
Added FHIR profile and related valuesets based on ZIB TextResult version 2017 - 4.1
</commit_message>
<xml_diff>
--- a/Mappings/TreatmentObjective - STU3.xlsx
+++ b/Mappings/TreatmentObjective - STU3.xlsx
@@ -300,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -344,6 +344,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -628,7 +631,7 @@
   <dimension ref="B2:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -718,14 +721,14 @@
     </row>
     <row r="4" spans="2:17" ht="63.75">
       <c r="B4" s="11"/>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
       <c r="G4" s="13"/>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="15" t="s">
         <v>15</v>
       </c>
       <c r="I4" s="2" t="s">
@@ -737,10 +740,10 @@
       <c r="K4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="M4" s="15" t="s">
         <v>20</v>
       </c>
       <c r="N4" s="2" t="s">
@@ -756,7 +759,7 @@
     </row>
     <row r="5" spans="2:17" ht="51">
       <c r="B5" s="11"/>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="12"/>
@@ -773,10 +776,10 @@
       <c r="K5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="M5" s="15" t="s">
         <v>26</v>
       </c>
       <c r="N5" s="2"/>
@@ -812,7 +815,7 @@
       <c r="L6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="M6" s="15" t="s">
         <v>31</v>
       </c>
       <c r="N6" s="2"/>
@@ -845,10 +848,10 @@
       <c r="K7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="L7" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="M7" s="15" t="s">
         <v>37</v>
       </c>
       <c r="N7" s="2"/>

</xml_diff>